<commit_message>
fixing 2022/02-Lacnov adding support for missing birth_years
</commit_message>
<xml_diff>
--- a/2022/01-brumov/01-VKCT2022-Brumov.xlsx
+++ b/2022/01-brumov/01-VKCT2022-Brumov.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="15"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Předškoláci I" sheetId="1" state="visible" r:id="rId2"/>
@@ -325,7 +325,7 @@
     <t xml:space="preserve">Mladší přípravka - dívky (2014-2015)</t>
   </si>
   <si>
-    <t xml:space="preserve">DULEČKOVÁ Kristýna</t>
+    <t xml:space="preserve">DOLEČKOVÁ Kristýna</t>
   </si>
   <si>
     <t xml:space="preserve">Bike Pro Racing</t>
@@ -661,7 +661,7 @@
     <t xml:space="preserve">Tufo CZ Otrokovice</t>
   </si>
   <si>
-    <t xml:space="preserve">ORSZÁKOVÁ Simona</t>
+    <t xml:space="preserve">ORSÁKOVÁ Simona</t>
   </si>
   <si>
     <t xml:space="preserve">Sport Club</t>
@@ -862,7 +862,7 @@
     <t xml:space="preserve">Karolinka</t>
   </si>
   <si>
-    <t xml:space="preserve">REHAK Ivan</t>
+    <t xml:space="preserve">REHÁK Ivan</t>
   </si>
   <si>
     <t xml:space="preserve">bike-centrum Dubnica</t>
@@ -985,7 +985,7 @@
     <t xml:space="preserve">Kolo Běžky</t>
   </si>
   <si>
-    <t xml:space="preserve">Jan Švehlik</t>
+    <t xml:space="preserve">Jan Švehlík</t>
   </si>
   <si>
     <t xml:space="preserve">Ženy – Klasik</t>
@@ -1357,7 +1357,7 @@
       <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.78515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.71"/>
@@ -2068,7 +2068,7 @@
       <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.78515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.71"/>
@@ -2581,11 +2581,11 @@
   </sheetPr>
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.78515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.71"/>
@@ -3081,7 +3081,7 @@
       <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.78515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.71"/>
@@ -3589,7 +3589,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.78515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.71"/>
@@ -4059,7 +4059,7 @@
       <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.78515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.71"/>
@@ -4526,10 +4526,10 @@
   <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
+      <selection pane="topLeft" activeCell="Q5" activeCellId="0" sqref="Q5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.78515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.71"/>
@@ -5257,11 +5257,11 @@
   </sheetPr>
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B30" activeCellId="0" sqref="B30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.78515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.71"/>
@@ -5884,10 +5884,10 @@
   <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
+      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.78515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.71"/>
@@ -6450,10 +6450,10 @@
   <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="J17" activeCellId="0" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.78515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.71"/>
@@ -6939,7 +6939,7 @@
       <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.78515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.71"/>
@@ -7829,7 +7829,7 @@
       <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.78515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.71"/>
@@ -8665,10 +8665,10 @@
   <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="I17" activeCellId="0" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.78515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.71"/>
@@ -9259,7 +9259,7 @@
       <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.78515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.71"/>
@@ -9749,10 +9749,10 @@
   <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.78515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.71"/>
@@ -10353,7 +10353,7 @@
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.78515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.71"/>
@@ -10916,7 +10916,7 @@
       <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.78515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.71"/>
@@ -11491,7 +11491,7 @@
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.78515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.71"/>
@@ -11969,10 +11969,10 @@
   <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+      <selection pane="topLeft" activeCell="I10" activeCellId="0" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.78515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.71"/>

</xml_diff>